<commit_message>
Update 04_Gant Chart Ver 1.2.xlsx
</commit_message>
<xml_diff>
--- a/src/04_Gant Chart Ver 1.2.xlsx
+++ b/src/04_Gant Chart Ver 1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MoneyManager_for_intel\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF68A67-C3B1-425B-9463-C17911C7500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D1F005-FC6B-4454-B2F9-2F95A52A20B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDA64757-50FA-684F-8087-8E7F312C180F}"/>
   </bookViews>
@@ -602,7 +602,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -660,25 +660,46 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -687,41 +708,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1040,11 +1037,11 @@
   <dimension ref="B1:AG64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="D2" sqref="D2"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6:B7"/>
+      <selection pane="bottomRight" activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1062,26 +1059,26 @@
   <sheetData>
     <row r="1" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:33" ht="38.25" x14ac:dyDescent="0.3">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D3" s="1"/>
@@ -1118,58 +1115,58 @@
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="21" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="23" t="s">
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="23" t="s">
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="23" t="s">
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="23" t="s">
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="21" t="s">
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AD6" s="21"/>
-      <c r="AE6" s="21"/>
-      <c r="AF6" s="21"/>
-      <c r="AG6" s="21"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="28"/>
     </row>
     <row r="7" spans="2:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="37"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="2">
         <v>44592</v>
       </c>
@@ -1262,10 +1259,10 @@
       </c>
     </row>
     <row r="8" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="9"/>
@@ -1300,9 +1297,9 @@
       <c r="AG8" s="12"/>
     </row>
     <row r="9" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="31"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -1334,8 +1331,8 @@
       <c r="AG9" s="15"/>
     </row>
     <row r="10" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31"/>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="29" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="11"/>
@@ -1370,8 +1367,8 @@
       <c r="AG10" s="12"/>
     </row>
     <row r="11" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="31"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="13"/>
@@ -1404,8 +1401,8 @@
       <c r="AG11" s="15"/>
     </row>
     <row r="12" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="31"/>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="29" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="11"/>
@@ -1440,8 +1437,8 @@
       <c r="AG12" s="12"/>
     </row>
     <row r="13" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="31"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -1474,8 +1471,8 @@
       <c r="AG13" s="15"/>
     </row>
     <row r="14" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="31"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="29" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="11"/>
@@ -1510,8 +1507,8 @@
       <c r="AG14" s="12"/>
     </row>
     <row r="15" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="31"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="16"/>
@@ -1544,10 +1541,10 @@
       <c r="AG15" s="15"/>
     </row>
     <row r="16" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="29" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="11"/>
@@ -1582,8 +1579,8 @@
       <c r="AG16" s="12"/>
     </row>
     <row r="17" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="31"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -1616,8 +1613,8 @@
       <c r="AG17" s="15"/>
     </row>
     <row r="18" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="31"/>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="29" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="11"/>
@@ -1652,8 +1649,8 @@
       <c r="AG18" s="12"/>
     </row>
     <row r="19" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="31"/>
-      <c r="C19" s="20"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
@@ -1686,8 +1683,8 @@
       <c r="AG19" s="15"/>
     </row>
     <row r="20" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="31"/>
-      <c r="C20" s="19" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="11"/>
@@ -1722,8 +1719,8 @@
       <c r="AG20" s="12"/>
     </row>
     <row r="21" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="31"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
@@ -1756,8 +1753,8 @@
       <c r="AG21" s="15"/>
     </row>
     <row r="22" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="31"/>
-      <c r="C22" s="19" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="29" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="11"/>
@@ -1792,8 +1789,8 @@
       <c r="AG22" s="12"/>
     </row>
     <row r="23" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="31"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
@@ -1826,8 +1823,8 @@
       <c r="AG23" s="15"/>
     </row>
     <row r="24" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="31"/>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="32"/>
+      <c r="C24" s="29" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="11"/>
@@ -1862,8 +1859,8 @@
       <c r="AG24" s="12"/>
     </row>
     <row r="25" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="31"/>
-      <c r="C25" s="20"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="30"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
@@ -1896,8 +1893,8 @@
       <c r="AG25" s="15"/>
     </row>
     <row r="26" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="31"/>
-      <c r="C26" s="19" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="29" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="11"/>
@@ -1932,8 +1929,8 @@
       <c r="AG26" s="12"/>
     </row>
     <row r="27" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="33"/>
-      <c r="C27" s="20"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
@@ -1966,10 +1963,10 @@
       <c r="AG27" s="15"/>
     </row>
     <row r="28" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D28" s="11"/>
@@ -2004,8 +2001,8 @@
       <c r="AG28" s="12"/>
     </row>
     <row r="29" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="31"/>
-      <c r="C29" s="20"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -2038,8 +2035,8 @@
       <c r="AG29" s="15"/>
     </row>
     <row r="30" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="31"/>
-      <c r="C30" s="19" t="s">
+      <c r="B30" s="32"/>
+      <c r="C30" s="29" t="s">
         <v>21</v>
       </c>
       <c r="D30" s="11"/>
@@ -2074,8 +2071,8 @@
       <c r="AG30" s="12"/>
     </row>
     <row r="31" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="31"/>
-      <c r="C31" s="20"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="30"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
@@ -2108,8 +2105,8 @@
       <c r="AG31" s="15"/>
     </row>
     <row r="32" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="31"/>
-      <c r="C32" s="19" t="s">
+      <c r="B32" s="32"/>
+      <c r="C32" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="11"/>
@@ -2144,8 +2141,8 @@
       <c r="AG32" s="12"/>
     </row>
     <row r="33" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="31"/>
-      <c r="C33" s="20"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
@@ -2178,8 +2175,8 @@
       <c r="AG33" s="15"/>
     </row>
     <row r="34" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="31"/>
-      <c r="C34" s="19" t="s">
+      <c r="B34" s="32"/>
+      <c r="C34" s="29" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="11"/>
@@ -2214,8 +2211,8 @@
       <c r="AG34" s="12"/>
     </row>
     <row r="35" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="33"/>
-      <c r="C35" s="20"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="30"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
@@ -2248,10 +2245,10 @@
       <c r="AG35" s="15"/>
     </row>
     <row r="36" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="11"/>
@@ -2286,8 +2283,8 @@
       <c r="AG36" s="12"/>
     </row>
     <row r="37" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="31"/>
-      <c r="C37" s="20"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="30"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
@@ -2301,7 +2298,7 @@
       <c r="N37" s="14"/>
       <c r="O37" s="14"/>
       <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
+      <c r="Q37" s="13"/>
       <c r="R37" s="14"/>
       <c r="S37" s="14"/>
       <c r="T37" s="14"/>
@@ -2320,8 +2317,8 @@
       <c r="AG37" s="15"/>
     </row>
     <row r="38" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="31"/>
-      <c r="C38" s="19" t="s">
+      <c r="B38" s="32"/>
+      <c r="C38" s="29" t="s">
         <v>21</v>
       </c>
       <c r="D38" s="11"/>
@@ -2338,7 +2335,7 @@
       <c r="O38" s="11"/>
       <c r="P38" s="11"/>
       <c r="Q38" s="11"/>
-      <c r="R38" s="29"/>
+      <c r="R38" s="11"/>
       <c r="S38" s="11"/>
       <c r="T38" s="11"/>
       <c r="U38" s="11"/>
@@ -2356,8 +2353,8 @@
       <c r="AG38" s="12"/>
     </row>
     <row r="39" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="31"/>
-      <c r="C39" s="20"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="30"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -2390,8 +2387,8 @@
       <c r="AG39" s="15"/>
     </row>
     <row r="40" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="31"/>
-      <c r="C40" s="19" t="s">
+      <c r="B40" s="32"/>
+      <c r="C40" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="11"/>
@@ -2426,8 +2423,8 @@
       <c r="AG40" s="12"/>
     </row>
     <row r="41" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="31"/>
-      <c r="C41" s="20"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="30"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
@@ -2460,8 +2457,8 @@
       <c r="AG41" s="15"/>
     </row>
     <row r="42" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="31"/>
-      <c r="C42" s="19" t="s">
+      <c r="B42" s="32"/>
+      <c r="C42" s="29" t="s">
         <v>41</v>
       </c>
       <c r="D42" s="11"/>
@@ -2496,8 +2493,8 @@
       <c r="AG42" s="12"/>
     </row>
     <row r="43" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="33"/>
-      <c r="C43" s="20"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="30"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
@@ -2530,10 +2527,10 @@
       <c r="AG43" s="15"/>
     </row>
     <row r="44" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="29" t="s">
         <v>25</v>
       </c>
       <c r="D44" s="11"/>
@@ -2568,8 +2565,8 @@
       <c r="AG44" s="12"/>
     </row>
     <row r="45" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="32"/>
-      <c r="C45" s="20"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="30"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
@@ -2602,8 +2599,8 @@
       <c r="AG45" s="15"/>
     </row>
     <row r="46" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="32"/>
-      <c r="C46" s="19" t="s">
+      <c r="B46" s="37"/>
+      <c r="C46" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D46" s="11"/>
@@ -2638,8 +2635,8 @@
       <c r="AG46" s="12"/>
     </row>
     <row r="47" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="32"/>
-      <c r="C47" s="20"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="30"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
@@ -2672,8 +2669,8 @@
       <c r="AG47" s="15"/>
     </row>
     <row r="48" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="32"/>
-      <c r="C48" s="19" t="s">
+      <c r="B48" s="37"/>
+      <c r="C48" s="29" t="s">
         <v>27</v>
       </c>
       <c r="D48" s="11"/>
@@ -2708,8 +2705,8 @@
       <c r="AG48" s="12"/>
     </row>
     <row r="49" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="32"/>
-      <c r="C49" s="20"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="30"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
@@ -2742,8 +2739,8 @@
       <c r="AG49" s="15"/>
     </row>
     <row r="50" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="32"/>
-      <c r="C50" s="19" t="s">
+      <c r="B50" s="37"/>
+      <c r="C50" s="29" t="s">
         <v>30</v>
       </c>
       <c r="D50" s="11"/>
@@ -2778,8 +2775,8 @@
       <c r="AG50" s="12"/>
     </row>
     <row r="51" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="35"/>
-      <c r="C51" s="20"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="30"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
@@ -2812,10 +2809,10 @@
       <c r="AG51" s="15"/>
     </row>
     <row r="52" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="29" t="s">
         <v>29</v>
       </c>
       <c r="D52" s="11"/>
@@ -2850,8 +2847,8 @@
       <c r="AG52" s="12"/>
     </row>
     <row r="53" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="31"/>
-      <c r="C53" s="20"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="30"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="14"/>
@@ -2884,8 +2881,8 @@
       <c r="AG53" s="15"/>
     </row>
     <row r="54" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="31"/>
-      <c r="C54" s="19" t="s">
+      <c r="B54" s="32"/>
+      <c r="C54" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D54" s="11"/>
@@ -2920,8 +2917,8 @@
       <c r="AG54" s="12"/>
     </row>
     <row r="55" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="31"/>
-      <c r="C55" s="20"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="30"/>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="14"/>
@@ -2954,8 +2951,8 @@
       <c r="AG55" s="15"/>
     </row>
     <row r="56" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="31"/>
-      <c r="C56" s="19" t="s">
+      <c r="B56" s="32"/>
+      <c r="C56" s="29" t="s">
         <v>42</v>
       </c>
       <c r="D56" s="11"/>
@@ -2990,8 +2987,8 @@
       <c r="AG56" s="12"/>
     </row>
     <row r="57" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="31"/>
-      <c r="C57" s="20"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="30"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="14"/>
@@ -3024,8 +3021,8 @@
       <c r="AG57" s="15"/>
     </row>
     <row r="58" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="31"/>
-      <c r="C58" s="19" t="s">
+      <c r="B58" s="32"/>
+      <c r="C58" s="29" t="s">
         <v>31</v>
       </c>
       <c r="D58" s="11"/>
@@ -3060,8 +3057,8 @@
       <c r="AG58" s="12"/>
     </row>
     <row r="59" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="31"/>
-      <c r="C59" s="20"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="30"/>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -3094,8 +3091,8 @@
       <c r="AG59" s="15"/>
     </row>
     <row r="60" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="31"/>
-      <c r="C60" s="19" t="s">
+      <c r="B60" s="32"/>
+      <c r="C60" s="29" t="s">
         <v>32</v>
       </c>
       <c r="D60" s="11"/>
@@ -3130,8 +3127,8 @@
       <c r="AG60" s="12"/>
     </row>
     <row r="61" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="33"/>
-      <c r="C61" s="20"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="30"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
@@ -3164,10 +3161,10 @@
       <c r="AG61" s="15"/>
     </row>
     <row r="62" spans="2:33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="30" t="s">
+      <c r="B62" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="29" t="s">
         <v>40</v>
       </c>
       <c r="D62" s="11"/>
@@ -3202,8 +3199,8 @@
       <c r="AG62" s="12"/>
     </row>
     <row r="63" spans="2:33" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="33"/>
-      <c r="C63" s="20"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="30"/>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
@@ -3271,29 +3268,16 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="D2:U2"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="S6:W6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="AC6:AG6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B44:B51"/>
-    <mergeCell ref="B16:B27"/>
-    <mergeCell ref="B28:B35"/>
-    <mergeCell ref="B36:B43"/>
-    <mergeCell ref="B52:B61"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C26:C27"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C38:C39"/>
@@ -3303,16 +3287,29 @@
     <mergeCell ref="C48:C49"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B44:B51"/>
+    <mergeCell ref="B16:B27"/>
+    <mergeCell ref="B28:B35"/>
+    <mergeCell ref="B36:B43"/>
+    <mergeCell ref="B52:B61"/>
+    <mergeCell ref="AC6:AG6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D2:U2"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="S6:W6"/>
+    <mergeCell ref="X6:AB6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>